<commit_message>
first week of 2025
</commit_message>
<xml_diff>
--- a/Webdesk-Journal-Export--jan.xlsx
+++ b/Webdesk-Journal-Export--jan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="111">
   <si>
     <t>Date</t>
   </si>
@@ -105,36 +105,33 @@
     <t/>
   </si>
   <si>
-    <t>08:12</t>
-  </si>
-  <si>
     <t>08:13</t>
   </si>
   <si>
+    <t>17:09</t>
+  </si>
+  <si>
+    <t>Homeoffice (20)</t>
+  </si>
+  <si>
     <t>8:00</t>
   </si>
   <si>
-    <t>8:27</t>
-  </si>
-  <si>
-    <t>17:07</t>
-  </si>
-  <si>
-    <t>0:27</t>
-  </si>
-  <si>
-    <t>9:27</t>
+    <t>8:26</t>
+  </si>
+  <si>
+    <t>17:06</t>
+  </si>
+  <si>
+    <t>0:26</t>
+  </si>
+  <si>
+    <t>9:26</t>
   </si>
   <si>
     <t>0:30</t>
   </si>
   <si>
-    <t>17:09</t>
-  </si>
-  <si>
-    <t>Homeoffice (20)</t>
-  </si>
-  <si>
     <t>Jan 3, 2025</t>
   </si>
   <si>
@@ -150,6 +147,21 @@
     <t>6:30</t>
   </si>
   <si>
+    <t>7:18</t>
+  </si>
+  <si>
+    <t>24:24</t>
+  </si>
+  <si>
+    <t>15:44</t>
+  </si>
+  <si>
+    <t>0:48</t>
+  </si>
+  <si>
+    <t>10:14</t>
+  </si>
+  <si>
     <t>Jan 4, 2025</t>
   </si>
   <si>
@@ -174,13 +186,106 @@
     <t>Tue</t>
   </si>
   <si>
+    <t>06:45</t>
+  </si>
+  <si>
+    <t>15:00</t>
+  </si>
+  <si>
+    <t>9:17</t>
+  </si>
+  <si>
+    <t>25:01</t>
+  </si>
+  <si>
+    <t>1:17</t>
+  </si>
+  <si>
+    <t>11:31</t>
+  </si>
+  <si>
+    <t>17:00</t>
+  </si>
+  <si>
+    <t>18:02</t>
+  </si>
+  <si>
     <t>Jan 8, 2025</t>
   </si>
   <si>
+    <t>7:45</t>
+  </si>
+  <si>
+    <t>17:02</t>
+  </si>
+  <si>
+    <t>32:46</t>
+  </si>
+  <si>
+    <t>-0:15</t>
+  </si>
+  <si>
+    <t>11:16</t>
+  </si>
+  <si>
     <t>Jan 9, 2025</t>
   </si>
   <si>
+    <t>08:10</t>
+  </si>
+  <si>
+    <t>9:06</t>
+  </si>
+  <si>
+    <t>26:08</t>
+  </si>
+  <si>
+    <t>41:52</t>
+  </si>
+  <si>
+    <t>1:06</t>
+  </si>
+  <si>
+    <t>12:22</t>
+  </si>
+  <si>
+    <t>17:43</t>
+  </si>
+  <si>
+    <t>19:15</t>
+  </si>
+  <si>
+    <t>mobile working (72)</t>
+  </si>
+  <si>
     <t>Jan 10, 2025</t>
+  </si>
+  <si>
+    <t>08:47</t>
+  </si>
+  <si>
+    <t>13:56</t>
+  </si>
+  <si>
+    <t>8:13</t>
+  </si>
+  <si>
+    <t>34:21</t>
+  </si>
+  <si>
+    <t>50:05</t>
+  </si>
+  <si>
+    <t>1:43</t>
+  </si>
+  <si>
+    <t>14:05</t>
+  </si>
+  <si>
+    <t>15:42</t>
+  </si>
+  <si>
+    <t>18:46</t>
   </si>
   <si>
     <t>Jan 11, 2025</t>
@@ -615,7 +720,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T33"/>
+  <dimension ref="A1:T35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -740,28 +845,28 @@
         <v>30</v>
       </c>
       <c r="G3">
-        <v>0.01</v>
+        <v>8.56</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
         <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" t="s">
         <v>33</v>
       </c>
-      <c r="M3" t="s">
-        <v>32</v>
-      </c>
       <c r="N3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O3" t="s">
         <v>24</v>
@@ -770,13 +875,13 @@
         <v>22</v>
       </c>
       <c r="Q3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R3">
         <v>0</v>
       </c>
       <c r="S3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="T3">
         <v>34.25</v>
@@ -784,370 +889,734 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4">
+        <v>7.48</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4" t="s">
         <v>37</v>
       </c>
-      <c r="G4">
-        <v>8.56</v>
-      </c>
-      <c r="H4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
+      <c r="T4">
+        <v>34.25</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5">
-        <v>7.48</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="J5" t="s">
-        <v>43</v>
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>47</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T5">
+        <v>34.25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" t="s">
         <v>44</v>
       </c>
-      <c r="B6" t="s">
+      <c r="M6" t="s">
         <v>45</v>
       </c>
-      <c r="J6" t="s">
-        <v>22</v>
+      <c r="N6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>47</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6" t="s">
+        <v>22</v>
+      </c>
+      <c r="T6">
+        <v>34.25</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q7" t="s">
         <v>47</v>
       </c>
-      <c r="J7" t="s">
-        <v>22</v>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7" t="s">
+        <v>22</v>
+      </c>
+      <c r="T7">
+        <v>34.25</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8">
+        <v>8.15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" t="s">
+        <v>28</v>
       </c>
       <c r="J8" t="s">
-        <v>22</v>
+        <v>32</v>
+      </c>
+      <c r="K8" t="s">
+        <v>58</v>
+      </c>
+      <c r="L8" t="s">
+        <v>58</v>
+      </c>
+      <c r="M8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N8" t="s">
+        <v>60</v>
+      </c>
+      <c r="O8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>61</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8" t="s">
+        <v>22</v>
+      </c>
+      <c r="T8">
+        <v>34.25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9">
+        <v>1.02</v>
+      </c>
+      <c r="H9" t="s">
         <v>31</v>
+      </c>
+      <c r="I9" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
         <v>21</v>
       </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10">
+        <v>8.15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" t="s">
+        <v>28</v>
+      </c>
       <c r="J10" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="K10" t="s">
+        <v>65</v>
+      </c>
+      <c r="L10" t="s">
+        <v>66</v>
+      </c>
+      <c r="M10" t="s">
+        <v>67</v>
+      </c>
+      <c r="N10" t="s">
+        <v>68</v>
+      </c>
+      <c r="O10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>69</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10" t="s">
+        <v>37</v>
+      </c>
+      <c r="T10">
+        <v>34.25</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
       </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11">
+        <v>7.34</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" t="s">
+        <v>28</v>
+      </c>
       <c r="J11" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="K11" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" t="s">
+        <v>73</v>
+      </c>
+      <c r="M11" t="s">
+        <v>74</v>
+      </c>
+      <c r="N11" t="s">
+        <v>75</v>
+      </c>
+      <c r="O11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>76</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11" t="s">
+        <v>22</v>
+      </c>
+      <c r="T11">
+        <v>34.25</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12" t="s">
-        <v>43</v>
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12">
+        <v>1.32</v>
+      </c>
+      <c r="H12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13">
+        <v>5.09</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" t="s">
+        <v>28</v>
       </c>
       <c r="J13" t="s">
-        <v>22</v>
+        <v>42</v>
+      </c>
+      <c r="K13" t="s">
+        <v>83</v>
+      </c>
+      <c r="L13" t="s">
+        <v>84</v>
+      </c>
+      <c r="M13" t="s">
+        <v>85</v>
+      </c>
+      <c r="N13" t="s">
+        <v>86</v>
+      </c>
+      <c r="O13" t="s">
+        <v>24</v>
+      </c>
+      <c r="P13" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>87</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13" t="s">
+        <v>22</v>
+      </c>
+      <c r="T13">
+        <v>34.25</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
-      </c>
-      <c r="J14" t="s">
-        <v>22</v>
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14">
+        <v>3.04</v>
+      </c>
+      <c r="H14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="B15" t="s">
         <v>49</v>
       </c>
       <c r="J15" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="B16" t="s">
         <v>51</v>
       </c>
       <c r="J16" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="J17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="J18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="J19" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="J20" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="J21" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="B22" t="s">
         <v>49</v>
       </c>
       <c r="J22" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="B23" t="s">
         <v>51</v>
       </c>
       <c r="J23" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="J24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="J25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="J26" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="J27" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="J28" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="B29" t="s">
         <v>49</v>
       </c>
       <c r="J29" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s">
         <v>51</v>
       </c>
       <c r="J30" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="J31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="J32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="J33" t="s">
-        <v>43</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+      <c r="J34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="J35" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:T33"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:T35"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>